<commit_message>
improve immutability of some path references
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED9D2A4-B1A3-4D6D-99DD-B46ABDB51FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C34D72-7806-4861-9DEC-9A6FAF40EAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="705" windowWidth="21217" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1338,6 +1338,22 @@
         <v>1.98</v>
       </c>
     </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="1">
+        <v>45875</v>
+      </c>
+      <c r="B119" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="1">
+        <v>45889</v>
+      </c>
+      <c r="B120" s="2">
+        <v>1.94</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update README, add slots to config .py files
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C34D72-7806-4861-9DEC-9A6FAF40EAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578A06F8-01FA-48FE-AD9D-71D944285EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="705" windowWidth="21217" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
+    <workbookView xWindow="750" yWindow="1087" windowWidth="21217" windowHeight="12593" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B120"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1354,6 +1354,14 @@
         <v>1.94</v>
       </c>
     </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="1">
+        <v>45898</v>
+      </c>
+      <c r="B121" s="2">
+        <v>1.82</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update uv; upgrade py and dependencies; add return_dtype= to polars .map(...)
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72908742-07EA-4810-96D7-40D1116A2220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF19728-DD1A-4B12-B609-4BA7A49D39EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{663B75C4-4EF0-43BA-B2A2-705907C78B86}"/>
   </bookViews>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23184F55-AF2F-421E-BC51-13A1C6FC6898}">
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1364,10 +1364,18 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
-        <v>45898</v>
+        <v>45909</v>
       </c>
       <c r="B122" s="2">
         <v>1.72</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B123" s="2">
+        <v>1.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update through update_data.py line 163
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47F6E86-7A65-4BB5-9638-BA7A0A1DED1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B6BCC3-92CC-48A4-A76F-F24F5E077C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B86" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1227,10 +1227,18 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92" s="4">
-        <v>45839</v>
+        <v>45930</v>
       </c>
       <c r="B92" s="2">
-        <v>1.78</v>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A93" s="4">
+        <v>45937</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update update_data.py through line 180
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B6BCC3-92CC-48A4-A76F-F24F5E077C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A71A5C-C561-408A-97A3-B3091ACC23BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3308" yWindow="1425" windowWidth="16620" windowHeight="11670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1241,6 +1241,14 @@
         <v>1.79</v>
       </c>
     </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A94" s="4">
+        <v>45937</v>
+      </c>
+      <c r="B94" s="2">
+        <v>1.76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update update_data.py through line 273
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A71A5C-C561-408A-97A3-B3091ACC23BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9669B6C0-B07A-4477-8E78-2E32789FE6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="1425" windowWidth="16620" windowHeight="11670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1243,10 +1243,18 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94" s="4">
-        <v>45937</v>
+        <v>45945</v>
       </c>
       <c r="B94" s="2">
         <v>1.76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95" s="4">
+        <v>45951</v>
+      </c>
+      <c r="B95" s="2">
+        <v>1.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all scripts and structure
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9669B6C0-B07A-4477-8E78-2E32789FE6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D1D87B-7560-49AE-A290-6DBE13578FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1470" windowWidth="23040" windowHeight="11670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1257,6 +1257,22 @@
         <v>1.7</v>
       </c>
     </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A96" s="4">
+        <v>45966</v>
+      </c>
+      <c r="B96" s="2">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A97" s="4">
+        <v>45973</v>
+      </c>
+      <c r="B97" s="2">
+        <v>1.81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fetch other indexes; add pl.Enum
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D1D87B-7560-49AE-A290-6DBE13578FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344089B9-556A-4139-B019-24899BB5ED1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1470" windowWidth="23040" windowHeight="11670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1837" windowWidth="23040" windowHeight="11670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <t>This data may be copyrighted. Please refer to the Terms of Use: https://fred.stlouisfed.org/legal#fred-terms-faq</t>
   </si>
   <si>
-    <t>File Created: 2025-09-22 3:18 pm CDT</t>
+    <t>File Created: 2025-12-05 12:55 pm CST</t>
   </si>
   <si>
     <t>DFII10</t>
@@ -47,7 +47,7 @@
     <t>Market Yield on U.S. Treasury Securities at 10-Year Constant Maturity, Quoted on an Investment Basis, Inflation-Indexed, Percent, Quarterly, Not Seasonally Adjusted</t>
   </si>
   <si>
-    <t>Data Updated: 2025-09-22</t>
+    <t>Data Updated: 2025-12-04</t>
   </si>
   <si>
     <t>observation_date</t>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92" s="4">
-        <v>45930</v>
+        <v>45839</v>
       </c>
       <c r="B92" s="2">
         <v>1.8</v>
@@ -1235,42 +1235,10 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" s="4">
-        <v>45937</v>
+        <v>45994</v>
       </c>
       <c r="B93" s="2">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A94" s="4">
-        <v>45945</v>
-      </c>
-      <c r="B94" s="2">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A95" s="4">
-        <v>45951</v>
-      </c>
-      <c r="B95" s="2">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A96" s="4">
-        <v>45966</v>
-      </c>
-      <c r="B96" s="2">
-        <v>1.87</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A97" s="4">
-        <v>45973</v>
-      </c>
-      <c r="B97" s="2">
-        <v>1.81</v>
+        <v>1.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidy env and param designs, part 1
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344089B9-556A-4139-B019-24899BB5ED1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB165C-989B-4972-9E1A-1242F9F27BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1837" windowWidth="23040" windowHeight="11670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="52" windowWidth="23040" windowHeight="13583" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1241,6 +1241,14 @@
         <v>1.82</v>
       </c>
     </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A94" s="4">
+        <v>46008</v>
+      </c>
+      <c r="B94" s="2">
+        <v>1.92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tidy architecture for read & write scripts
</commit_message>
<xml_diff>
--- a/input_output/input_dir/DFII10.xlsx
+++ b/input_output/input_dir/DFII10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Python_Projects\sp500_earn_price_pkg\input_output\input_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB165C-989B-4972-9E1A-1242F9F27BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD0D863-468E-405B-A5BF-9779D9187185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="52" windowWidth="23040" windowHeight="13583" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="52" windowWidth="22673" windowHeight="13583" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1249,6 +1249,30 @@
         <v>1.92</v>
       </c>
     </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95" s="4">
+        <v>46022</v>
+      </c>
+      <c r="B95" s="2">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A96" s="4">
+        <v>46031</v>
+      </c>
+      <c r="B96" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A97" s="4">
+        <v>46038</v>
+      </c>
+      <c r="B97" s="2">
+        <v>1.89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>